<commit_message>
Hr question are added
</commit_message>
<xml_diff>
--- a/Hr-Calls-Questions.xlsx
+++ b/Hr-Calls-Questions.xlsx
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>